<commit_message>
added id column to templates
</commit_message>
<xml_diff>
--- a/input_templates/example_address.xlsx
+++ b/input_templates/example_address.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rutger.Hofste\Documents\GitHub\aqueduct_analyze_locations\input_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D7103071-993C-4054-811F-12CB193A485A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{081E089B-7727-4614-81BA-ACFD782F985A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{189EB58F-33CB-43D4-A517-2AEAA424F687}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>location name</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Fluwelen Burgwal 58, 2511 CJ, The Hague, Netherlands</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -425,45 +428,57 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5C9A599-2174-40F6-B6EA-7A7F1A3E5746}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="74.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="74.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add id column to xlsx
</commit_message>
<xml_diff>
--- a/input_templates/example_address.xlsx
+++ b/input_templates/example_address.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rutger.Hofste\Documents\GitHub\aqueduct_analyze_locations\input_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{081E089B-7727-4614-81BA-ACFD782F985A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{55F3BF9B-0130-44FC-9967-39444E26D19A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{189EB58F-33CB-43D4-A517-2AEAA424F687}"/>
   </bookViews>
@@ -430,7 +430,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5C9A599-2174-40F6-B6EA-7A7F1A3E5746}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>